<commit_message>
Test Commit First Try Biemel GruppeA
</commit_message>
<xml_diff>
--- a/SCRUM/SCRUM_TEAM_A.xlsx
+++ b/SCRUM/SCRUM_TEAM_A.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57553D62-1D17-463E-B854-9E0DE57067CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>PO - Backlog</t>
   </si>
@@ -99,12 +100,15 @@
   </si>
   <si>
     <t>Due: 04.11.2021</t>
+  </si>
+  <si>
+    <t>Test f. Commit Biemel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -587,22 +591,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="65.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -624,7 +628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -636,7 +640,7 @@
       </c>
       <c r="D3" s="12"/>
     </row>
-    <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -648,7 +652,7 @@
       </c>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -660,7 +664,7 @@
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -672,7 +676,7 @@
       </c>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>2</v>
       </c>
@@ -684,7 +688,7 @@
       </c>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -696,7 +700,7 @@
       </c>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -708,7 +712,7 @@
       </c>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>2</v>
       </c>
@@ -720,7 +724,7 @@
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>3</v>
       </c>
@@ -732,235 +736,235 @@
       </c>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="13"/>
     </row>
-    <row r="18" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="19" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="13"/>
     </row>
-    <row r="23" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="25" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="13"/>
     </row>
-    <row r="39" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="13"/>
     </row>
-    <row r="42" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="13"/>
     </row>
-    <row r="46" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="13"/>
     </row>
-    <row r="47" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="13"/>
     </row>
-    <row r="48" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="13"/>
     </row>
-    <row r="50" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -972,23 +976,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D4"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="65.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1010,7 +1014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1024,7 +1028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1038,282 +1042,287 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="13"/>
     </row>
-    <row r="18" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="19" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="13"/>
     </row>
-    <row r="23" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="25" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="13"/>
     </row>
-    <row r="39" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="13"/>
     </row>
-    <row r="42" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="13"/>
     </row>
-    <row r="46" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="13"/>
     </row>
-    <row r="47" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="13"/>
     </row>
-    <row r="48" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="13"/>
     </row>
-    <row r="50" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
       <c r="D50" s="13"/>
     </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test 1 Commit Scherer
</commit_message>
<xml_diff>
--- a/SCRUM/SCRUM_TEAM_A.xlsx
+++ b/SCRUM/SCRUM_TEAM_A.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57553D62-1D17-463E-B854-9E0DE57067CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{57553D62-1D17-463E-B854-9E0DE57067CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35C7A022-3706-4F49-91A7-7492EBC0B961}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="2940" windowWidth="14580" windowHeight="9982" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>PO - Backlog</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Test f. Commit Biemel</t>
+  </si>
+  <si>
+    <t>Test f. Commit Scherer</t>
   </si>
 </sst>
 </file>
@@ -598,15 +601,15 @@
       <selection activeCell="A3" sqref="A3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.86328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="65.86328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.73046875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +617,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -628,7 +631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -640,7 +643,7 @@
       </c>
       <c r="D3" s="12"/>
     </row>
-    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -652,7 +655,7 @@
       </c>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -664,7 +667,7 @@
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -676,7 +679,7 @@
       </c>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>2</v>
       </c>
@@ -688,7 +691,7 @@
       </c>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -700,7 +703,7 @@
       </c>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -712,7 +715,7 @@
       </c>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
         <v>2</v>
       </c>
@@ -724,7 +727,7 @@
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7">
         <v>3</v>
       </c>
@@ -736,235 +739,235 @@
       </c>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="7"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="7"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="7"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="13"/>
     </row>
-    <row r="18" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="7"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="19" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="7"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="7"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="7"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="7"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="13"/>
     </row>
-    <row r="23" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="7"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="7"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="25" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="7"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="7"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="7"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="7"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="7"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="7"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="7"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="7"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="7"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="7"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="7"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="7"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="7"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="7"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="13"/>
     </row>
-    <row r="39" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="7"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="7"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="7"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="13"/>
     </row>
-    <row r="42" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="7"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="7"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="7"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="7"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="13"/>
     </row>
-    <row r="46" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="7"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="13"/>
     </row>
-    <row r="47" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="7"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="13"/>
     </row>
-    <row r="48" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="7"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="7"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="13"/>
     </row>
-    <row r="50" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A50" s="8"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -977,22 +980,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.86328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="65.86328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.73046875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1042,285 +1045,290 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="7"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="7"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="7"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="7"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="13"/>
     </row>
-    <row r="18" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="7"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="19" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="7"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="7"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="7"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="7"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="13"/>
     </row>
-    <row r="23" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="7"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="7"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="25" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="7"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="7"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="7"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="7"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="7"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="7"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="7"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="7"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="7"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="7"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="7"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="7"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="7"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="7"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="13"/>
     </row>
-    <row r="39" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="7"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="7"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="7"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="13"/>
     </row>
-    <row r="42" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="7"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="7"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="7"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="7"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="13"/>
     </row>
-    <row r="46" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="7"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="13"/>
     </row>
-    <row r="47" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="7"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="13"/>
     </row>
-    <row r="48" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="7"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="7"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="13"/>
     </row>
-    <row r="50" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A50" s="8"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
       <c r="D50" s="13"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rückgängig Test Biemel Scherer
</commit_message>
<xml_diff>
--- a/SCRUM/SCRUM_TEAM_A.xlsx
+++ b/SCRUM/SCRUM_TEAM_A.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{57553D62-1D17-463E-B854-9E0DE57067CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99033B4B-335D-4374-BC4E-9EF79D6F5623}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{57553D62-1D17-463E-B854-9E0DE57067CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A17BDA0C-2F43-4413-B884-DA362EB901F1}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="2940" windowWidth="14580" windowHeight="9982" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>PO - Backlog</t>
   </si>
@@ -100,12 +100,6 @@
   </si>
   <si>
     <t>Due: 04.11.2021</t>
-  </si>
-  <si>
-    <t>Test f. Commit Biemel</t>
-  </si>
-  <si>
-    <t>2. Test f. Commit Scherer</t>
   </si>
 </sst>
 </file>
@@ -980,10 +974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1321,16 +1315,6 @@
       <c r="C50" s="11"/>
       <c r="D50" s="13"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A52" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Vorhandene Interfaces niemals ändern! Stattdessen erweitern bzw. davon ableiten!
</commit_message>
<xml_diff>
--- a/SCRUM/SCRUM_TEAM_A.xlsx
+++ b/SCRUM/SCRUM_TEAM_A.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>PO - Backlog</t>
   </si>
@@ -59,27 +59,15 @@
     <t>Implementierung der TicTacToe-Darstellung</t>
   </si>
   <si>
-    <t>Umsetzung des Painters im Framework.</t>
-  </si>
-  <si>
     <t>Implementierung der TicTacToe-Regeln</t>
   </si>
   <si>
-    <t>Umsetzung der Rules im Framework.</t>
-  </si>
-  <si>
     <t>Implementierung eines menschlichen TicTacToe-Spielers</t>
   </si>
   <si>
-    <t>Umsetzung eines menschlichen Players im Framework.</t>
-  </si>
-  <si>
     <t>Implementierung eines PC gesteurten TicTacToe-Spielers</t>
   </si>
   <si>
-    <t>Umsetzung eines PC gesteuerten Players im Framework.</t>
-  </si>
-  <si>
     <t>Spezifikation eines weiteren Spiels</t>
   </si>
   <si>
@@ -99,6 +87,36 @@
   </si>
   <si>
     <t>Due: 04.11.2021</t>
+  </si>
+  <si>
+    <t>10min</t>
+  </si>
+  <si>
+    <t>Umsetzung des Painters im Framework: Standard TicTacToe. Mit Ausblick auf Animation und Schattierung. Schwarzes Gitter, blaue Kreuze, rote Kreise.</t>
+  </si>
+  <si>
+    <t>Umsetzung eines menschlichen Players im Framework: Standard TicTacToe mit Mausbedingung. Mit Ausblick auf Namen eingeben</t>
+  </si>
+  <si>
+    <t>Highscore Umsetzung und Darstellung im Framework Integrieren/Spezifizieren.</t>
+  </si>
+  <si>
+    <t>Highscore: Wo, wie darstellen? Wo, wie speichern? Wie wo umsetzen?</t>
+  </si>
+  <si>
+    <t>Umsetzung der Rules im Framework: Standard TicTacToe mit 30s Zeitlimit. Mit Ausblick auf Highscore. Gewinn +1 Punkt, Verlieren -2 Punkte.</t>
+  </si>
+  <si>
+    <t>Umsetzung eines PC gesteuerten Players im Framework: Standard TicTacToe.</t>
+  </si>
+  <si>
+    <t>Focus-Faktor: 0,5</t>
+  </si>
+  <si>
+    <t>180min</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -267,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -307,6 +325,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +628,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -668,7 +689,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D6" s="13"/>
     </row>
@@ -677,10 +698,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D7" s="13"/>
     </row>
@@ -689,10 +710,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D8" s="13"/>
     </row>
@@ -701,10 +722,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D9" s="13"/>
     </row>
@@ -713,10 +734,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D10" s="13"/>
     </row>
@@ -725,17 +746,23 @@
         <v>3</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="7">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -973,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,15 +1015,18 @@
     <col min="5" max="5" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1010,7 +1040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1021,10 +1051,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1035,76 +1068,106 @@
         <v>7</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>

</xml_diff>

<commit_message>
Planung 11.11.2021 Gruppe A, B und D
</commit_message>
<xml_diff>
--- a/SCRUM/SCRUM_TEAM_A.xlsx
+++ b/SCRUM/SCRUM_TEAM_A.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55149F01-19B4-407C-BD7D-CF076670B8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>PO - Backlog</t>
   </si>
@@ -51,12 +50,6 @@
     <t>Visual Studio, TortoiseGit, GitHub, Anaoconda (ML) testen und installieren.</t>
   </si>
   <si>
-    <t>Spezifikation einer Umsetzungsidee für das Spiel TicTacToe</t>
-  </si>
-  <si>
-    <t>Spezifikation: Wie soll das TicTacToe aussehen? Wie soll das Aussehen technisch erreicht werden? Wie sollen Regeln umgesetzt werden? Soll es Sonderregeln geben, bzw. Sonderspielfelder, etc.? Welche Spieler (PC, ...) soll es geben? Etc.?</t>
-  </si>
-  <si>
     <t>Implementierung der TicTacToe-Darstellung</t>
   </si>
   <si>
@@ -81,18 +74,6 @@
     <t>Umsetzung eines PC gesteuerten Players im Framework.</t>
   </si>
   <si>
-    <t>Spezifikation eines weiteren Spiels</t>
-  </si>
-  <si>
-    <t>Im Entwicklungsteam kann beschlossen werden welches weitere Spiel umgesetzt werden soll, bzw. kann.</t>
-  </si>
-  <si>
-    <t>Erzeugung der TicTacToe-Spieler in einer Fabrik.</t>
-  </si>
-  <si>
-    <t>Umsetung einer Fabrik zur Erzeugung der menschlichen und PC gesteuerten TicTacToe-Spieler.</t>
-  </si>
-  <si>
     <t>Sprint - Backlog</t>
   </si>
   <si>
@@ -100,12 +81,45 @@
   </si>
   <si>
     <t>Due: 04.11.2021</t>
+  </si>
+  <si>
+    <t>180min</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>60min</t>
+  </si>
+  <si>
+    <t>120min</t>
+  </si>
+  <si>
+    <t>Time-Limit</t>
+  </si>
+  <si>
+    <t>Name für Spieler</t>
+  </si>
+  <si>
+    <t>Eingabe der Namen für die einzelnen Spieler.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time-Limit für Spielzüge bei TicTacToe. </t>
+  </si>
+  <si>
+    <t>Spezifikation neues Spiel</t>
+  </si>
+  <si>
+    <t>Spezifikation neues Spiel.</t>
+  </si>
+  <si>
+    <t>Überplant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -268,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -308,6 +322,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,30 +605,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C4"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="65.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -625,343 +642,319 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>8</v>
-      </c>
+    <row r="3" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="12"/>
     </row>
-    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>7</v>
-      </c>
+    <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>2</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>10</v>
-      </c>
+    <row r="5" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>2</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>12</v>
-      </c>
+    <row r="6" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>2</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>14</v>
-      </c>
+    <row r="7" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>2</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>2</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
         <v>3</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="13"/>
     </row>
-    <row r="18" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="19" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="13"/>
     </row>
-    <row r="23" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="25" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="13"/>
     </row>
-    <row r="39" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="13"/>
     </row>
-    <row r="42" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="13"/>
     </row>
-    <row r="46" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="13"/>
     </row>
-    <row r="47" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="13"/>
     </row>
-    <row r="48" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="13"/>
     </row>
-    <row r="50" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="8"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -973,31 +966,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="65.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1011,7 +1004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1022,10 +1015,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1036,280 +1032,354 @@
         <v>7</v>
       </c>
       <c r="D4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7"/>
+    </row>
+    <row r="8" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8"/>
+    </row>
+    <row r="9" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9"/>
+    </row>
+    <row r="10" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>2</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>3</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="13"/>
     </row>
-    <row r="18" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="19" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="13"/>
     </row>
-    <row r="23" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="25" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="13"/>
     </row>
-    <row r="39" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="13"/>
     </row>
-    <row r="42" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="13"/>
     </row>
-    <row r="46" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="13"/>
     </row>
-    <row r="47" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="13"/>
     </row>
-    <row r="48" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="13"/>
     </row>
-    <row r="50" spans="1:4" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="8"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>

</xml_diff>